<commit_message>
fix and update tests, fix delete test data
</commit_message>
<xml_diff>
--- a/src/test/java/me/iskrone/w2r4s/data/TestBooks.xlsx
+++ b/src/test/java/me/iskrone/w2r4s/data/TestBooks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\w2r4s_github\src\test\java\me\iskrone\w2r4s\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Автор</t>
   </si>
@@ -45,9 +42,6 @@
     <t>Gordon Ramsay</t>
   </si>
   <si>
-    <t>6 Кулинария</t>
-  </si>
-  <si>
     <t>Нет</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>Трое в лодке не считая собаки</t>
   </si>
   <si>
-    <t>Художественная</t>
-  </si>
-  <si>
     <t>да</t>
   </si>
   <si>
@@ -91,6 +82,9 @@
   </si>
   <si>
     <t>audio</t>
+  </si>
+  <si>
+    <t>TEST_TEST_TEST</t>
   </si>
 </sst>
 </file>
@@ -409,24 +403,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,82 +437,79 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1">
+        <v>38718</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="G4" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1">
-        <v>38718</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>